<commit_message>
should be good. waiting on request limit to chill
</commit_message>
<xml_diff>
--- a/SpotifyArtists.xlsx
+++ b/SpotifyArtists.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
         <v>82</v>
       </c>
       <c r="F2" t="n">
-        <v>12251558</v>
+        <v>12255907</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -519,7 +519,7 @@
         <v>86</v>
       </c>
       <c r="F3" t="n">
-        <v>15101494</v>
+        <v>15105758</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -550,7 +550,7 @@
         <v>83</v>
       </c>
       <c r="F4" t="n">
-        <v>8130231</v>
+        <v>8134833</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -581,7 +581,7 @@
         <v>90</v>
       </c>
       <c r="F5" t="n">
-        <v>13903566</v>
+        <v>13911352</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -612,7 +612,7 @@
         <v>84</v>
       </c>
       <c r="F6" t="n">
-        <v>8327152</v>
+        <v>8331177</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
         <v>74</v>
       </c>
       <c r="F7" t="n">
-        <v>5881125</v>
+        <v>5881585</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -657,28 +657,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Schoolboy Q</t>
+          <t>21 Savage</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ScHoolboy Q</t>
+          <t>21 Savage</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>spotify:artist:5IcR3N7QB1j6KBL8eImZ8m</t>
+          <t>spotify:artist:1URnnhqYAYcrqrcwql10ft</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F8" t="n">
-        <v>4496035</v>
+        <v>13714232</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['gangster rap', 'hip hop', 'pop rap', 'rap', 'southern hip hop', 'trap']</t>
+          <t>['atl hip hop', 'hip hop', 'rap', 'trap']</t>
         </is>
       </c>
     </row>
@@ -688,28 +688,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>21 Savage</t>
+          <t>Lil Wayne</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>21 Savage</t>
+          <t>Lil Wayne</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>spotify:artist:1URnnhqYAYcrqrcwql10ft</t>
+          <t>spotify:artist:55Aa2cqylxrFIXC767Z865</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F9" t="n">
-        <v>13706173</v>
+        <v>13566338</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['atl hip hop', 'hip hop', 'rap', 'trap']</t>
+          <t>['hip hop', 'new orleans rap', 'pop rap', 'rap', 'trap']</t>
         </is>
       </c>
     </row>
@@ -719,28 +719,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lil Wayne</t>
+          <t>Drake</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lil Wayne</t>
+          <t>Drake</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>spotify:artist:55Aa2cqylxrFIXC767Z865</t>
+          <t>spotify:artist:3TVXtAsR1Inumwj472S9r4</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F10" t="n">
-        <v>13562233</v>
+        <v>75402118</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['hip hop', 'new orleans rap', 'pop rap', 'rap', 'trap']</t>
+          <t>['canadian hip hop', 'canadian pop', 'hip hop', 'rap', 'toronto rap']</t>
         </is>
       </c>
     </row>
@@ -750,28 +750,28 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Drake</t>
+          <t>Travis Scott</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Drake</t>
+          <t>Travis Scott</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>spotify:artist:3TVXtAsR1Inumwj472S9r4</t>
+          <t>spotify:artist:0Y5tJX1MQlPlqiwlOH1tJY</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F11" t="n">
-        <v>75373513</v>
+        <v>22467114</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['canadian hip hop', 'canadian pop', 'hip hop', 'rap', 'toronto rap']</t>
+          <t>['hip hop', 'rap', 'slap house']</t>
         </is>
       </c>
     </row>
@@ -781,28 +781,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Travis Scott</t>
+          <t>Juice WRLD</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Travis Scott</t>
+          <t>Juice WRLD</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>spotify:artist:0Y5tJX1MQlPlqiwlOH1tJY</t>
+          <t>spotify:artist:4MCBfE4596Uoi2O4DtmEMz</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12" t="n">
-        <v>22461051</v>
+        <v>29163755</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['hip hop', 'rap', 'slap house']</t>
+          <t>['chicago rap', 'melodic rap', 'rap']</t>
         </is>
       </c>
     </row>
@@ -812,28 +812,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Juice WRLD</t>
+          <t>J. Cole</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Juice WRLD</t>
+          <t>J. Cole</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>spotify:artist:4MCBfE4596Uoi2O4DtmEMz</t>
+          <t>spotify:artist:6l3HvQ5sa6mXTsMTB19rO5</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" t="n">
-        <v>29151420</v>
+        <v>20174199</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['chicago rap', 'melodic rap', 'rap']</t>
+          <t>['conscious hip hop', 'hip hop', 'north carolina hip hop', 'rap']</t>
         </is>
       </c>
     </row>
@@ -843,28 +843,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>J. Cole</t>
+          <t>Lil Baby</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>J. Cole</t>
+          <t>Lil Baby</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>spotify:artist:6l3HvQ5sa6mXTsMTB19rO5</t>
+          <t>spotify:artist:5f7VJjfbwm532GiveGC0ZK</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F14" t="n">
-        <v>20164337</v>
+        <v>14164707</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['conscious hip hop', 'hip hop', 'north carolina hip hop', 'rap']</t>
+          <t>['atl hip hop', 'atl trap', 'rap', 'trap']</t>
         </is>
       </c>
     </row>
@@ -874,28 +874,28 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lil Baby</t>
+          <t>Kendrick Lamar</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Lil Baby</t>
+          <t>Kendrick Lamar</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>spotify:artist:5f7VJjfbwm532GiveGC0ZK</t>
+          <t>spotify:artist:2YZyLoL8N0Wb9xBt1NhZWg</t>
         </is>
       </c>
       <c r="E15" t="n">
         <v>89</v>
       </c>
       <c r="F15" t="n">
-        <v>14154233</v>
+        <v>24034094</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['atl hip hop', 'atl trap', 'rap', 'trap']</t>
+          <t>['conscious hip hop', 'hip hop', 'rap', 'west coast rap']</t>
         </is>
       </c>
     </row>
@@ -905,28 +905,28 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DaBaby</t>
+          <t>Roddy Ricch</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>DaBaby</t>
+          <t>Roddy Ricch</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>spotify:artist:4r63FhuTkUYltbVAg5TQnk</t>
+          <t>spotify:artist:757aE44tKEUQEqRuT6GnEB</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F16" t="n">
-        <v>10816327</v>
+        <v>9355580</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['hip hop', 'north carolina hip hop', 'rap']</t>
+          <t>['melodic rap', 'rap', 'trap']</t>
         </is>
       </c>
     </row>
@@ -936,28 +936,28 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Kendrick Lamar</t>
+          <t>Meek Mill</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Kendrick Lamar</t>
+          <t>Meek Mill</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>spotify:artist:2YZyLoL8N0Wb9xBt1NhZWg</t>
+          <t>spotify:artist:20sxb77xiYeusSH8cVdatc</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F17" t="n">
-        <v>24021239</v>
+        <v>7227194</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['conscious hip hop', 'hip hop', 'rap', 'west coast rap']</t>
+          <t>['hip hop', 'philly rap', 'pop rap', 'rap', 'southern hip hop', 'trap']</t>
         </is>
       </c>
     </row>
@@ -967,28 +967,28 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Roddy Ricch</t>
+          <t>Kanye West</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Roddy Ricch</t>
+          <t>Kanye West</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>spotify:artist:757aE44tKEUQEqRuT6GnEB</t>
+          <t>spotify:artist:5K4W6rqBFWDnAN6FQUkS6x</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F18" t="n">
-        <v>9351978</v>
+        <v>20119636</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['melodic rap', 'rap', 'trap']</t>
+          <t>['chicago rap', 'hip hop', 'rap']</t>
         </is>
       </c>
     </row>
@@ -998,28 +998,28 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Meek Mill</t>
+          <t>JAY-Z</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Meek Mill</t>
+          <t>JAY-Z</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>spotify:artist:20sxb77xiYeusSH8cVdatc</t>
+          <t>spotify:artist:3nFkdlSjzX9mRTtwJOzDYB</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F19" t="n">
-        <v>7224077</v>
+        <v>8372130</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>['hip hop', 'philly rap', 'pop rap', 'rap', 'southern hip hop', 'trap']</t>
+          <t>['east coast hip hop', 'gangster rap', 'hip hop', 'pop rap', 'rap']</t>
         </is>
       </c>
     </row>
@@ -1029,28 +1029,28 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kanye West</t>
+          <t>Isaiah Rashad</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Kanye West</t>
+          <t>Isaiah Rashad</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>spotify:artist:5K4W6rqBFWDnAN6FQUkS6x</t>
+          <t>spotify:artist:6aaMZ3fcfLv4tEbmY7bjRM</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="F20" t="n">
-        <v>20110972</v>
+        <v>1280375</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>['chicago rap', 'hip hop', 'rap']</t>
+          <t>['hip hop', 'indie hip hop', 'rap', 'tennessee hip hop', 'underground hip hop']</t>
         </is>
       </c>
     </row>
@@ -1060,28 +1060,28 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>JAY-Z</t>
+          <t>Eminem</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>JAY-Z</t>
+          <t>Eminem</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>spotify:artist:3nFkdlSjzX9mRTtwJOzDYB</t>
+          <t>spotify:artist:7dGJo4pcD2V6oG8kP0tJRR</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F21" t="n">
-        <v>8369956</v>
+        <v>70916249</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>['east coast hip hop', 'gangster rap', 'hip hop', 'pop rap', 'rap']</t>
+          <t>['detroit hip hop', 'hip hop', 'rap']</t>
         </is>
       </c>
     </row>
@@ -1091,28 +1091,28 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Isaiah Rashad</t>
+          <t>Pop Smoke</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Isaiah Rashad</t>
+          <t>Pop Smoke</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>spotify:artist:6aaMZ3fcfLv4tEbmY7bjRM</t>
+          <t>spotify:artist:0eDvMgVFoNV3TpwtrVCoTj</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="F22" t="n">
-        <v>1280000</v>
+        <v>12496140</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>['hip hop', 'indie hip hop', 'rap', 'tennessee hip hop', 'underground hip hop']</t>
+          <t>['brooklyn drill', 'rap']</t>
         </is>
       </c>
     </row>
@@ -1122,28 +1122,28 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Eminem</t>
+          <t>Lil Durk</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Eminem</t>
+          <t>Lil Durk</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>spotify:artist:7dGJo4pcD2V6oG8kP0tJRR</t>
+          <t>spotify:artist:3hcs9uc56yIGFCSy9leWe7</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F23" t="n">
-        <v>70867094</v>
+        <v>5572550</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>['detroit hip hop', 'hip hop', 'rap']</t>
+          <t>['chicago drill', 'chicago rap', 'drill', 'hip hop', 'rap', 'trap']</t>
         </is>
       </c>
     </row>
@@ -1153,28 +1153,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pop Smoke</t>
+          <t>Gunna</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Pop Smoke</t>
+          <t>Gunna</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>spotify:artist:0eDvMgVFoNV3TpwtrVCoTj</t>
+          <t>spotify:artist:2hlmm7s2ICUX0LVIhVFlZQ</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F24" t="n">
-        <v>12492198</v>
+        <v>5266687</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>['brooklyn drill', 'rap']</t>
+          <t>['atl hip hop', 'melodic rap', 'rap', 'trap']</t>
         </is>
       </c>
     </row>
@@ -1184,28 +1184,28 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Lil Durk</t>
+          <t>Trippie Redd</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Lil Durk</t>
+          <t>Trippie Redd</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>spotify:artist:3hcs9uc56yIGFCSy9leWe7</t>
+          <t>spotify:artist:6Xgp2XMz1fhVYe7i6yNAax</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F25" t="n">
-        <v>5565846</v>
+        <v>8685735</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>['chicago drill', 'chicago rap', 'drill', 'hip hop', 'rap', 'trap']</t>
+          <t>['melodic rap', 'rap']</t>
         </is>
       </c>
     </row>
@@ -1215,28 +1215,28 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A Boogie wit da Hoodie</t>
+          <t>Kid Cudi</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>A Boogie Wit da Hoodie</t>
+          <t>Kid Cudi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>spotify:artist:31W5EY0aAly4Qieq6OFu6I</t>
+          <t>spotify:artist:0fA0VVWsXO9YnASrzqfmYu</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F26" t="n">
-        <v>7412812</v>
+        <v>6485796</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>['melodic rap', 'rap', 'trap']</t>
+          <t>['hip hop', 'ohio hip hop', 'pop rap', 'rap']</t>
         </is>
       </c>
     </row>
@@ -1246,28 +1246,28 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Gunna</t>
+          <t>Pusha T</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Gunna</t>
+          <t>Pusha T</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>spotify:artist:2hlmm7s2ICUX0LVIhVFlZQ</t>
+          <t>spotify:artist:0ONHkAv9pCAFxb0zJwDNTy</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="F27" t="n">
-        <v>5264026</v>
+        <v>2766333</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>['atl hip hop', 'melodic rap', 'rap', 'trap']</t>
+          <t>['gangster rap', 'hip hop', 'rap', 'southern hip hop', 'trap', 'virginia hip hop']</t>
         </is>
       </c>
     </row>
@@ -1277,28 +1277,28 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Migos</t>
+          <t>Earl Sweatshirt</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Migos</t>
+          <t>Earl Sweatshirt</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>spotify:artist:6oMuImdp5ZcFhWP0ESe6mG</t>
+          <t>spotify:artist:3A5tHz1SfngyOZM2gItYKu</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F28" t="n">
-        <v>13176525</v>
+        <v>2012650</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>['atl hip hop', 'hip hop', 'rap', 'trap']</t>
+          <t>['drumless hip hop', 'experimental hip hop', 'hip hop', 'rap', 'underground hip hop']</t>
         </is>
       </c>
     </row>
@@ -1308,28 +1308,28 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Trippie Redd</t>
+          <t>Tyler, The Creator</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Trippie Redd</t>
+          <t>Tyler, The Creator</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>spotify:artist:6Xgp2XMz1fhVYe7i6yNAax</t>
+          <t>spotify:artist:4V8LLVI7PbaPR0K2TGSxFF</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F29" t="n">
-        <v>8683281</v>
+        <v>11528855</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>['melodic rap', 'rap']</t>
+          <t>['hip hop', 'rap']</t>
         </is>
       </c>
     </row>
@@ -1339,28 +1339,28 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Kid Cudi</t>
+          <t>Big Sean</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Kid Cudi</t>
+          <t>Big Sean</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>spotify:artist:0fA0VVWsXO9YnASrzqfmYu</t>
+          <t>spotify:artist:0c173mlxpT3dSFRgMO8XPh</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F30" t="n">
-        <v>6484371</v>
+        <v>10821493</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>['hip hop', 'ohio hip hop', 'pop rap', 'rap']</t>
+          <t>['detroit hip hop', 'hip hop', 'pop rap', 'r&amp;b', 'rap', 'southern hip hop', 'trap']</t>
         </is>
       </c>
     </row>
@@ -1370,28 +1370,28 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Pusha T</t>
+          <t>Yeat</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Pusha T</t>
+          <t>Yeat</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>spotify:artist:0ONHkAv9pCAFxb0zJwDNTy</t>
+          <t>spotify:artist:3qiHUAX7zY4Qnjx8TNUzVx</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F31" t="n">
-        <v>2765580</v>
+        <v>2451174</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>['gangster rap', 'hip hop', 'rap', 'southern hip hop', 'trap', 'virginia hip hop']</t>
+          <t>['pluggnb', 'rage rap']</t>
         </is>
       </c>
     </row>
@@ -1401,28 +1401,28 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Earl Sweatshirt</t>
+          <t>Don Toliver</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Earl Sweatshirt</t>
+          <t>Don Toliver</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>spotify:artist:3A5tHz1SfngyOZM2gItYKu</t>
+          <t>spotify:artist:4Gso3d4CscCijv0lmajZWs</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="F32" t="n">
-        <v>2012034</v>
+        <v>2887244</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>['drumless hip hop', 'experimental hip hop', 'hip hop', 'rap', 'underground hip hop']</t>
+          <t>['rap']</t>
         </is>
       </c>
     </row>
@@ -1432,28 +1432,28 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Tyler, The Creator</t>
+          <t>Migos</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tyler, The Creator</t>
+          <t>Migos</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>spotify:artist:4V8LLVI7PbaPR0K2TGSxFF</t>
+          <t>spotify:artist:6oMuImdp5ZcFhWP0ESe6mG</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F33" t="n">
-        <v>11519172</v>
+        <v>13178912</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>['hip hop', 'rap']</t>
+          <t>['atl hip hop', 'hip hop', 'rap', 'trap']</t>
         </is>
       </c>
     </row>
@@ -1463,586 +1463,28 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Big Sean</t>
+          <t>Action Bronson</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Big Sean</t>
+          <t>Action Bronson</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>spotify:artist:0c173mlxpT3dSFRgMO8XPh</t>
+          <t>spotify:artist:7BMccF0hQFBpP6417k1OtQ</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="F34" t="n">
-        <v>10824411</v>
+        <v>764128</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>['detroit hip hop', 'hip hop', 'pop rap', 'r&amp;b', 'rap', 'southern hip hop', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Yeat</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Yeat</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>spotify:artist:3qiHUAX7zY4Qnjx8TNUzVx</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>83</v>
-      </c>
-      <c r="F35" t="n">
-        <v>2445948</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>['pluggnb', 'rage rap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Ken Carson</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Ken Carson</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>spotify:artist:3gBZUcNeVumkeeJ19CY2sX</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>71</v>
-      </c>
-      <c r="F36" t="n">
-        <v>492136</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>['rage rap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Destroy Lonely</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Destroy Lonely</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>spotify:artist:1HPW4jeRjXBFRoUnSvBzoD</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>77</v>
-      </c>
-      <c r="F37" t="n">
-        <v>498157</v>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>['rage rap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Saba</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Saba</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>spotify:artist:7Hjbimq43OgxaBRpFXic4x</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>64</v>
-      </c>
-      <c r="F38" t="n">
-        <v>679888</v>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>['alternative r&amp;b', 'chicago rap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>6lack</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>6LACK</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>spotify:artist:4IVAbR2w4JJNJDDRFP3E83</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>76</v>
-      </c>
-      <c r="F39" t="n">
-        <v>4227680</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>['atl hip hop', 'melodic rap', 'r&amp;b', 'rap', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>JID</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>JID</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>spotify:artist:6U3ybJ9UHNKEdsH7ktGBZ7</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
-        <v>77</v>
-      </c>
-      <c r="F40" t="n">
-        <v>1221273</v>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>['hip hop', 'rap', 'underground hip hop']</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Bad Bunny</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Bad Bunny</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>spotify:artist:4q3ewBCX7sLwd24euuV69X</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>97</v>
-      </c>
-      <c r="F41" t="n">
-        <v>69374424</v>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>['reggaeton', 'trap latino', 'urbano latino']</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Don Toliver</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Don Toliver</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>spotify:artist:4Gso3d4CscCijv0lmajZWs</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>84</v>
-      </c>
-      <c r="F42" t="n">
-        <v>2884733</v>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>['rap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Metro Boomin</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Metro Boomin</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>spotify:artist:0iEtIxbK0KxaSlF7G42ZOp</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>89</v>
-      </c>
-      <c r="F43" t="n">
-        <v>4319285</v>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>['rap', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Offset</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Offset</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>spotify:artist:4DdkRBBYG6Yk9Ka8tdJ9BW</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>78</v>
-      </c>
-      <c r="F44" t="n">
-        <v>2761605</v>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>['atl hip hop', 'rap', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Quavo</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Quavo</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>spotify:artist:0VRj0yCOv2FXJNP47XQnx5</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>80</v>
-      </c>
-      <c r="F45" t="n">
-        <v>6611403</v>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>['atl hip hop', 'melodic rap', 'rap', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Takeoff</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Takeoff</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>spotify:artist:3EW0kQ1skZiK1NHg3Spt9J</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>72</v>
-      </c>
-      <c r="F46" t="n">
-        <v>1412108</v>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>['atl hip hop', 'rap', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Migos</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Migos</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>spotify:artist:6oMuImdp5ZcFhWP0ESe6mG</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>77</v>
-      </c>
-      <c r="F47" t="n">
-        <v>13176525</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>['atl hip hop', 'hip hop', 'rap', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Key Glock</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Key Glock</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>spotify:artist:0RESbWvOMyua0yuyVrztJ5</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>75</v>
-      </c>
-      <c r="F48" t="n">
-        <v>1582592</v>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>['memphis hip hop', 'tennessee hip hop', 'trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Young Nudy</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Young Nudy</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>spotify:artist:5yPzzu25VzEk8qrGTLIrE1</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>72</v>
-      </c>
-      <c r="F49" t="n">
-        <v>1159979</v>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>['pluggnb', 'rap', 'trap', 'vapor trap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Action Bronson</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Action Bronson</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>spotify:artist:7BMccF0hQFBpP6417k1OtQ</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>63</v>
-      </c>
-      <c r="F50" t="n">
-        <v>764010</v>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
           <t>['alternative hip hop', 'east coast hip hop', 'hip hop', 'nyc rap', 'queens hip hop']</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Larry June</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Larry June</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>spotify:artist:1grN0519h2zYqpRtYbDZAl</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>67</v>
-      </c>
-      <c r="F51" t="n">
-        <v>273140</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>['cali rap']</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>The Alchemist</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>The Alchemist</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>spotify:artist:0eVyjRhzZKke2KFYTcDkeu</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>72</v>
-      </c>
-      <c r="F52" t="n">
-        <v>461820</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>['alternative hip hop', 'drumless hip hop', 'hip hop', 'instrumental hip hop', 'west coast rap']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
should run all 4 in succession (metrics once a week)
</commit_message>
<xml_diff>
--- a/SpotifyArtists.xlsx
+++ b/SpotifyArtists.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>genres</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -488,11 +493,16 @@
         <v>82</v>
       </c>
       <c r="F2" t="n">
-        <v>12255907</v>
+        <v>12264838</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>['east coast hip hop', 'hip hop', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebee452efcf24aa4124fb28d94</t>
         </is>
       </c>
     </row>
@@ -519,11 +529,16 @@
         <v>86</v>
       </c>
       <c r="F3" t="n">
-        <v>15105758</v>
+        <v>15114832</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>['melodic rap', 'philly rap', 'rage rap', 'rap']</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb30122c0d3ead72f96bb5ee93</t>
         </is>
       </c>
     </row>
@@ -550,11 +565,16 @@
         <v>83</v>
       </c>
       <c r="F4" t="n">
-        <v>8134833</v>
+        <v>8144120</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>['atl hip hop', 'plugg', 'pluggnb', 'rage rap', 'rap']</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb504ff11d788162fbf8078654</t>
         </is>
       </c>
     </row>
@@ -581,11 +601,16 @@
         <v>90</v>
       </c>
       <c r="F5" t="n">
-        <v>13911352</v>
+        <v>13928327</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>['atl hip hop', 'hip hop', 'rap', 'southern hip hop', 'trap']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb24e41f491b129093a6fee383</t>
         </is>
       </c>
     </row>
@@ -612,11 +637,16 @@
         <v>84</v>
       </c>
       <c r="F6" t="n">
-        <v>8331177</v>
+        <v>8340304</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>['atl hip hop', 'atl trap', 'gangster rap', 'melodic rap', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb547d2b41c9f2c97318aad0ed</t>
         </is>
       </c>
     </row>
@@ -643,11 +673,16 @@
         <v>74</v>
       </c>
       <c r="F7" t="n">
-        <v>5881585</v>
+        <v>5882877</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>['chicago rap', 'conscious hip hop', 'hip hop', 'pop rap', 'rap']</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eba6ab3c4df02cec59758ae3fa</t>
         </is>
       </c>
     </row>
@@ -674,11 +709,16 @@
         <v>91</v>
       </c>
       <c r="F8" t="n">
-        <v>13714232</v>
+        <v>13731066</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>['atl hip hop', 'hip hop', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb35ca7d2181258b51c0f2cf9e</t>
         </is>
       </c>
     </row>
@@ -702,14 +742,19 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" t="n">
-        <v>13566338</v>
+        <v>13575711</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>['hip hop', 'new orleans rap', 'pop rap', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebc63aded6f4bf4d06d1377106</t>
         </is>
       </c>
     </row>
@@ -736,11 +781,16 @@
         <v>96</v>
       </c>
       <c r="F10" t="n">
-        <v>75402118</v>
+        <v>75467555</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>['canadian hip hop', 'canadian pop', 'hip hop', 'rap', 'toronto rap']</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb4293385d324db8558179afd9</t>
         </is>
       </c>
     </row>
@@ -767,11 +817,16 @@
         <v>90</v>
       </c>
       <c r="F11" t="n">
-        <v>22467114</v>
+        <v>22479986</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>['hip hop', 'rap', 'slap house']</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebe707b87e3f65997f6c09bfff</t>
         </is>
       </c>
     </row>
@@ -798,11 +853,16 @@
         <v>88</v>
       </c>
       <c r="F12" t="n">
-        <v>29163755</v>
+        <v>29189277</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
           <t>['chicago rap', 'melodic rap', 'rap']</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb1908e1a8b79abf71d5598944</t>
         </is>
       </c>
     </row>
@@ -829,11 +889,16 @@
         <v>87</v>
       </c>
       <c r="F13" t="n">
-        <v>20174199</v>
+        <v>20194806</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>['conscious hip hop', 'hip hop', 'north carolina hip hop', 'rap']</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebadd503b411a712e277895c8a</t>
         </is>
       </c>
     </row>
@@ -860,11 +925,16 @@
         <v>89</v>
       </c>
       <c r="F14" t="n">
-        <v>14164707</v>
+        <v>14188438</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>['atl hip hop', 'atl trap', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb6cad3eff5adc29e20f189a6c</t>
         </is>
       </c>
     </row>
@@ -891,11 +961,16 @@
         <v>89</v>
       </c>
       <c r="F15" t="n">
-        <v>24034094</v>
+        <v>24059100</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
           <t>['conscious hip hop', 'hip hop', 'rap', 'west coast rap']</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb437b9e2a82505b3d93ff1022</t>
         </is>
       </c>
     </row>
@@ -922,11 +997,16 @@
         <v>80</v>
       </c>
       <c r="F16" t="n">
-        <v>9355580</v>
+        <v>9363182</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
           <t>['melodic rap', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb9c30c6b69a55d48decd71600</t>
         </is>
       </c>
     </row>
@@ -953,11 +1033,16 @@
         <v>75</v>
       </c>
       <c r="F17" t="n">
-        <v>7227194</v>
+        <v>7234151</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>['hip hop', 'philly rap', 'pop rap', 'rap', 'southern hip hop', 'trap']</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb238b2a30c741d42a4c91b7b7</t>
         </is>
       </c>
     </row>
@@ -984,11 +1069,16 @@
         <v>90</v>
       </c>
       <c r="F18" t="n">
-        <v>20119636</v>
+        <v>20137321</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
           <t>['chicago rap', 'hip hop', 'rap']</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb867008a971fae0f4d913f63a</t>
         </is>
       </c>
     </row>
@@ -1015,11 +1105,16 @@
         <v>84</v>
       </c>
       <c r="F19" t="n">
-        <v>8372130</v>
+        <v>8376711</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
           <t>['east coast hip hop', 'gangster rap', 'hip hop', 'pop rap', 'rap']</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebc75afcd5a9027f60eaebb5e4</t>
         </is>
       </c>
     </row>
@@ -1046,11 +1141,16 @@
         <v>67</v>
       </c>
       <c r="F20" t="n">
-        <v>1280375</v>
+        <v>1281076</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>['hip hop', 'indie hip hop', 'rap', 'tennessee hip hop', 'underground hip hop']</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb1ff1685224034e6c12538722</t>
         </is>
       </c>
     </row>
@@ -1077,11 +1177,16 @@
         <v>91</v>
       </c>
       <c r="F21" t="n">
-        <v>70916249</v>
+        <v>71020309</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
           <t>['detroit hip hop', 'hip hop', 'rap']</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eba00b11c129b27a88fc72f36b</t>
         </is>
       </c>
     </row>
@@ -1108,11 +1213,16 @@
         <v>82</v>
       </c>
       <c r="F22" t="n">
-        <v>12496140</v>
+        <v>12504534</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
           <t>['brooklyn drill', 'rap']</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb597f9edd2cd1a892d4412b09</t>
         </is>
       </c>
     </row>
@@ -1136,14 +1246,19 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F23" t="n">
-        <v>5572550</v>
+        <v>5589335</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
           <t>['chicago drill', 'chicago rap', 'drill', 'hip hop', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eba0461c1f2218374aa672ce4e</t>
         </is>
       </c>
     </row>
@@ -1170,11 +1285,16 @@
         <v>84</v>
       </c>
       <c r="F24" t="n">
-        <v>5266687</v>
+        <v>5272350</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
           <t>['atl hip hop', 'melodic rap', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb803f228472451496cb2f5b88</t>
         </is>
       </c>
     </row>
@@ -1201,11 +1321,16 @@
         <v>81</v>
       </c>
       <c r="F25" t="n">
-        <v>8685735</v>
+        <v>8690894</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
           <t>['melodic rap', 'rap']</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb32f8f4df5e7b05a7e4d170ca</t>
         </is>
       </c>
     </row>
@@ -1232,11 +1357,16 @@
         <v>80</v>
       </c>
       <c r="F26" t="n">
-        <v>6485796</v>
+        <v>6488601</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
           <t>['hip hop', 'ohio hip hop', 'pop rap', 'rap']</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb876faa285687786c3d314ae0</t>
         </is>
       </c>
     </row>
@@ -1263,11 +1393,16 @@
         <v>71</v>
       </c>
       <c r="F27" t="n">
-        <v>2766333</v>
+        <v>2767861</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
           <t>['gangster rap', 'hip hop', 'rap', 'southern hip hop', 'trap', 'virginia hip hop']</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebc5b88a3924d8318f25f20594</t>
         </is>
       </c>
     </row>
@@ -1294,11 +1429,16 @@
         <v>69</v>
       </c>
       <c r="F28" t="n">
-        <v>2012650</v>
+        <v>2013768</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
           <t>['drumless hip hop', 'experimental hip hop', 'hip hop', 'rap', 'underground hip hop']</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb5e93db92ca7864585fbe5f28</t>
         </is>
       </c>
     </row>
@@ -1325,11 +1465,16 @@
         <v>88</v>
       </c>
       <c r="F29" t="n">
-        <v>11528855</v>
+        <v>11548636</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
           <t>['hip hop', 'rap']</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb8278b782cbb5a3963db88ada</t>
         </is>
       </c>
     </row>
@@ -1356,11 +1501,16 @@
         <v>77</v>
       </c>
       <c r="F30" t="n">
-        <v>10821493</v>
+        <v>10818217</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
           <t>['detroit hip hop', 'hip hop', 'pop rap', 'r&amp;b', 'rap', 'southern hip hop', 'trap']</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eb89dccc0a0b3d818c8d5fb711</t>
         </is>
       </c>
     </row>
@@ -1387,11 +1537,16 @@
         <v>83</v>
       </c>
       <c r="F31" t="n">
-        <v>2451174</v>
+        <v>2462095</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
           <t>['pluggnb', 'rage rap']</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5eba36d13951ab8280a63bac16c</t>
         </is>
       </c>
     </row>
@@ -1418,11 +1573,16 @@
         <v>84</v>
       </c>
       <c r="F32" t="n">
-        <v>2887244</v>
+        <v>2892760</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
           <t>['rap']</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebeb63bf6379a9ea8453a30020</t>
         </is>
       </c>
     </row>
@@ -1449,11 +1609,16 @@
         <v>77</v>
       </c>
       <c r="F33" t="n">
-        <v>13178912</v>
+        <v>13184018</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
           <t>['atl hip hop', 'hip hop', 'rap', 'trap']</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebf4593f7b778219838d858c34</t>
         </is>
       </c>
     </row>
@@ -1480,11 +1645,16 @@
         <v>63</v>
       </c>
       <c r="F34" t="n">
-        <v>764128</v>
+        <v>764444</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
           <t>['alternative hip hop', 'east coast hip hop', 'hip hop', 'nyc rap', 'queens hip hop']</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab6761610000e5ebaef8392a62c123944b6383b2</t>
         </is>
       </c>
     </row>

</xml_diff>